<commit_message>
Workin on sampletab conversion
</commit_message>
<xml_diff>
--- a/t/data/Excel/sampleset.bsamples.xlsx
+++ b/t/data/Excel/sampleset.bsamples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="612" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37460" windowHeight="15860" tabRatio="612" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -707,7 +707,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="291">
+  <cellStyleXfs count="293">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -986,6 +986,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1035,7 +1037,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="291">
+  <cellStyles count="293">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1221,6 +1223,8 @@
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2198,7 +2202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -2733,7 +2737,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D1810" sqref="D1810"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2825,16 +2831,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
         <v>130</v>
       </c>
@@ -2848,25 +2856,25 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>135</v>
       </c>
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
       <c r="D2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17">
+    <row r="3" spans="1:4" ht="17">
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
     </row>
-    <row r="4" spans="1:5" ht="17">
+    <row r="4" spans="1:4" ht="17">
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
     </row>

</xml_diff>

<commit_message>
working on the SampleTab conversion
</commit_message>
<xml_diff>
--- a/t/data/Excel/sampleset.bsamples.xlsx
+++ b/t/data/Excel/sampleset.bsamples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37460" windowHeight="15860" tabRatio="612" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37460" windowHeight="15860" tabRatio="612" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -319,9 +319,6 @@
     <t>Delivery ease</t>
   </si>
   <si>
-    <t>Term source REF</t>
-  </si>
-  <si>
     <t>Physiological conditions</t>
   </si>
   <si>
@@ -503,6 +500,9 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/BTO_0000214</t>
+  </si>
+  <si>
+    <t>Derived from</t>
   </si>
 </sst>
 </file>
@@ -1723,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1752,7 +1752,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>24</v>
+        <v>157</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>4</v>
@@ -1770,7 +1770,7 @@
         <v>42</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>43</v>
@@ -1793,13 +1793,13 @@
         <v>84</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2"/>
       <c r="I2" s="12" t="s">
@@ -1826,13 +1826,13 @@
         <v>62</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3"/>
       <c r="I3" s="12" t="s">
@@ -2270,7 +2270,7 @@
         <v>6</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>72</v>
@@ -2750,34 +2750,34 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
         <v>123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>124</v>
       </c>
       <c r="D2">
         <v>1.2</v>
@@ -2804,19 +2804,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2833,7 +2833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2844,30 +2844,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
         <v>134</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>135</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>136</v>
-      </c>
-      <c r="D2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17">
@@ -2899,10 +2899,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>139</v>
       </c>
       <c r="C1" s="6"/>
     </row>
@@ -2926,13 +2926,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2950,20 +2950,20 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2971,7 +2971,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2979,7 +2979,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2987,7 +2987,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2995,7 +2995,7 @@
         <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3003,31 +3003,31 @@
         <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" t="s">
         <v>150</v>
-      </c>
-      <c r="B7" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s">
         <v>153</v>
-      </c>
-      <c r="B9" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3035,7 +3035,7 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3043,7 +3043,7 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3051,7 +3051,7 @@
         <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3068,8 +3068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AT1" sqref="AT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3226,25 +3226,25 @@
         <v>41</v>
       </c>
       <c r="AM1" s="6" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="AN1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AO1" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP1" s="6" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="AQ1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="AR1" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AS1" s="6" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="AT1" s="7" t="s">
         <v>6</v>
@@ -3314,17 +3314,17 @@
       <c r="AK2" s="14"/>
       <c r="AL2" s="4"/>
       <c r="AM2" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AN2" s="15"/>
       <c r="AO2" s="4"/>
       <c r="AP2" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AQ2" s="15"/>
       <c r="AR2" s="4"/>
       <c r="AS2" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AT2" s="15"/>
     </row>
@@ -3414,7 +3414,7 @@
   <dimension ref="A1:AF125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3459,7 +3459,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>24</v>
+        <v>157</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>4</v>
@@ -3483,7 +3483,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>22</v>
@@ -3492,7 +3492,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>9</v>
@@ -3516,10 +3516,10 @@
         <v>6</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X1" s="6" t="s">
         <v>5</v>
@@ -3528,22 +3528,22 @@
         <v>6</v>
       </c>
       <c r="Z1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AB1" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:32">
@@ -3557,13 +3557,13 @@
         <v>19</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="13" t="s">
@@ -3609,7 +3609,7 @@
         <v>57</v>
       </c>
       <c r="X2" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AF2" s="26"/>
     </row>
@@ -3624,13 +3624,13 @@
         <v>20</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="13" t="s">
@@ -3679,13 +3679,13 @@
         <v>21</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="13" t="s">

</xml_diff>

<commit_message>
clean up term source IDs
</commit_message>
<xml_diff>
--- a/t/data/Excel/sampleset.bsamples.xlsx
+++ b/t/data/Excel/sampleset.bsamples.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="3240" windowWidth="38400" windowHeight="9540" tabRatio="612" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="612" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="162">
   <si>
     <t>NCBI Taxonomy</t>
   </si>
@@ -508,7 +508,13 @@
     <t>EFO_0001265</t>
   </si>
   <si>
-    <t>CL_0000542</t>
+    <t>OBI:0001468</t>
+  </si>
+  <si>
+    <t>NCBITaxon_9796</t>
+  </si>
+  <si>
+    <t>CL:0000542</t>
   </si>
 </sst>
 </file>
@@ -1848,7 +1854,7 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="G3"/>
       <c r="I3" s="12" t="s">
@@ -1861,7 +1867,7 @@
         <v>43</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -3095,7 +3101,7 @@
   <dimension ref="A1:AT3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3377,8 +3383,8 @@
       <c r="H3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="9">
-        <v>9796</v>
+      <c r="I3" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="9"/>

</xml_diff>